<commit_message>
m - update code
</commit_message>
<xml_diff>
--- a/ExcelSheet/RetailerChannel.xlsx
+++ b/ExcelSheet/RetailerChannel.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" date1904="false" showObjects="all"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="4" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="827" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="9" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="827" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="TestCase" r:id="rId2" sheetId="1" state="visible"/>
@@ -17,13 +17,15 @@
     <sheet name="CreateRetailer" r:id="rId8" sheetId="7" state="visible"/>
     <sheet name="AddDistributor" r:id="rId9" sheetId="8" state="visible"/>
     <sheet name="AddRetailer" r:id="rId10" sheetId="9" state="visible"/>
+    <sheet name="CheckRetailerBalance" r:id="rId11" sheetId="10" state="visible"/>
+    <sheet name="EditRetailer" r:id="rId12" sheetId="11" state="visible"/>
   </sheets>
   <calcPr iterate="false" iterateCount="100" iterateDelta="0.001" refMode="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="60">
   <si>
     <t>TCID</t>
   </si>
@@ -49,6 +51,9 @@
     <t>RetailerTransfer</t>
   </si>
   <si>
+    <t>Pass</t>
+  </si>
+  <si>
     <t>RetailerBalanceReport</t>
   </si>
   <si>
@@ -64,9 +69,18 @@
     <t>AddDistributor</t>
   </si>
   <si>
+    <t>Fail</t>
+  </si>
+  <si>
     <t>AddRetailer</t>
   </si>
   <si>
+    <t>CheckRetailerBalance</t>
+  </si>
+  <si>
+    <t>EditRetailer</t>
+  </si>
+  <si>
     <t>Actual Result</t>
   </si>
   <si>
@@ -103,9 +117,6 @@
     <t>Successfully transfered the Amount</t>
   </si>
   <si>
-    <t>Pass</t>
-  </si>
-  <si>
     <t>710100052</t>
   </si>
   <si>
@@ -118,10 +129,7 @@
     <t>710100042</t>
   </si>
   <si>
-    <t>Retailer Nummber Mismatched</t>
-  </si>
-  <si>
-    <t>Fail</t>
+    <t>Retailer Amount matched</t>
   </si>
   <si>
     <t>7101000521</t>
@@ -187,10 +195,17 @@
     <t>azsx1234</t>
   </si>
   <si>
-    <t>Retailer Amount matched</t>
+    <t>retailerNu</t>
   </si>
   <si>
     <t/>
+  </si>
+  <si>
+    <t>Establishment great00785</t>
+  </si>
+  <si>
+    <t>Establishment great00785: 7101000521
+ Current Balance is Rs. 66.25</t>
   </si>
 </sst>
 </file>
@@ -200,7 +215,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -235,6 +250,11 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -292,7 +312,7 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="44">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
@@ -313,6 +333,10 @@
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
       <protection hidden="false" locked="true"/>
     </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
     <xf applyAlignment="true" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
       <protection hidden="false" locked="true"/>
@@ -325,13 +349,49 @@
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="false" applyProtection="false" borderId="1" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
     <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="5" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="2" fontId="6" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment wrapText="true"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment wrapText="true"/>
@@ -413,10 +473,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100">
-      <selection activeCell="D4" activeCellId="0" pane="topLeft" sqref="D4"/>
+      <selection activeCell="B11" activeCellId="0" pane="topLeft" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -462,24 +522,24 @@
       <c r="B3" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="18" t="s">
-        <v>26</v>
+      <c r="D3" s="5" t="s">
+        <v>8</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="4">
       <c r="A4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="5" t="s">
         <v>8</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="21" t="s">
-        <v>26</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="5">
       <c r="A5" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B5" s="0" t="s">
         <v>6</v>
@@ -487,7 +547,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="6">
       <c r="A6" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B6" s="0" t="s">
         <v>6</v>
@@ -496,29 +556,48 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="7">
       <c r="A7" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B7" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="5"/>
+      <c r="D7" s="6"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="8">
       <c r="A8" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B8" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="30" t="s">
-        <v>32</v>
+      <c r="D8" s="5" t="s">
+        <v>14</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="9">
       <c r="A9" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B9" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="10">
+      <c r="A10" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="43" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="11">
+      <c r="A11" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="0" t="s">
         <v>6</v>
       </c>
     </row>
@@ -526,6 +605,147 @@
   <printOptions gridLines="false" gridLinesSet="true" headings="false" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins bottom="1.05277777777778" footer="0.7875" header="0.7875" left="0.7875" right="0.7875" top="1.05277777777778"/>
   <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="1" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="true" usePrinterDefaults="false" verticalDpi="300"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100">
+      <selection activeCell="G1" activeCellId="0" pane="topLeft" sqref="G1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col min="1" max="1" hidden="false" style="0" width="11.5204081632653" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" hidden="false" style="0" width="23.0859375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" hidden="false" style="0" width="6.171875" collapsed="true"/>
+    <col min="4" max="1025" hidden="false" style="0" width="11.5204081632653" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2">
+      <c r="A2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="42" t="s">
+        <v>59</v>
+      </c>
+      <c r="C2" s="41" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions gridLines="false" gridLinesSet="true" headings="false" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins bottom="1.05277777777778" footer="0.7875" header="0.7875" left="0.7875" right="0.7875" top="1.05277777777778"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100">
+      <selection activeCell="I29" activeCellId="0" pane="topLeft" sqref="I29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col min="1" max="1025" hidden="false" style="0" width="11.5204081632653" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2">
+      <c r="A2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions gridLines="false" gridLinesSet="true" headings="false" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins bottom="1.05277777777778" footer="0.7875" header="0.7875" left="0.7875" right="0.7875" top="1.05277777777778"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -557,38 +777,38 @@
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1" s="6" t="s">
+      <c r="B1" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="7" t="s">
         <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2">
       <c r="A2" s="3" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="3" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -610,14 +830,14 @@
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100">
-      <selection activeCell="H4" activeCellId="0" pane="topLeft" sqref="H4"/>
+      <selection activeCell="E1" activeCellId="0" pane="topLeft" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col min="1" max="1" hidden="false" style="0" width="11.5204081632653" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" hidden="false" style="0" width="30.75390625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" hidden="false" style="0" width="6.171875" collapsed="true"/>
+    <col min="2" max="2" hidden="false" style="0" width="30.75" collapsed="true"/>
+    <col min="3" max="3" hidden="false" style="0" width="6.1734693877551" collapsed="true"/>
     <col min="4" max="7" hidden="false" style="0" width="11.5204081632653" collapsed="true"/>
     <col min="8" max="8" hidden="false" style="0" width="13.75" collapsed="true"/>
     <col min="9" max="1025" hidden="false" style="0" width="11.5204081632653" collapsed="true"/>
@@ -627,56 +847,56 @@
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1" s="6" t="s">
+      <c r="B1" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="7" t="s">
         <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2">
       <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="C2" s="16" t="s">
-        <v>26</v>
+      <c r="B2" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="3" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -714,29 +934,29 @@
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1" s="7" t="s">
+      <c r="B1" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="8" t="s">
         <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2">
@@ -747,19 +967,19 @@
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
       <c r="E2" s="3" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -780,15 +1000,15 @@
   </sheetPr>
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100">
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100">
       <selection activeCell="G2" activeCellId="0" pane="topLeft" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col min="1" max="1" hidden="false" style="0" width="11.5204081632653" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" hidden="false" style="0" width="22.40625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" hidden="false" style="0" width="6.171875" collapsed="true"/>
+    <col min="2" max="2" hidden="false" style="0" width="22.4081632653061" collapsed="true"/>
+    <col min="3" max="3" hidden="false" style="0" width="6.1734693877551" collapsed="true"/>
     <col min="4" max="7" hidden="false" style="0" width="11.5204081632653" collapsed="true"/>
     <col min="8" max="8" hidden="false" style="0" width="13.75" collapsed="true"/>
     <col min="9" max="1025" hidden="false" style="0" width="11.5204081632653" collapsed="true"/>
@@ -798,50 +1018,50 @@
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1" s="6" t="s">
+      <c r="B1" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="7" t="s">
         <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2">
       <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="20" t="s">
-        <v>54</v>
-      </c>
-      <c r="C2" s="19" t="s">
-        <v>26</v>
+      <c r="B2" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="3" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -878,26 +1098,26 @@
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1" s="6" t="s">
+      <c r="B1" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="7" t="s">
         <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2">
@@ -905,23 +1125,23 @@
         <v>6</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="3" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -958,56 +1178,56 @@
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1" s="6" t="s">
+      <c r="B1" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="7" t="s">
         <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="18" outlineLevel="0" r="2">
       <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>26</v>
+      <c r="B2" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>8</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="3" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -1035,8 +1255,8 @@
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col min="1" max="1" hidden="false" style="0" width="11.5204081632653" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" hidden="false" style="0" width="11.953125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" hidden="false" style="0" width="6.171875" collapsed="true"/>
+    <col min="2" max="2" hidden="false" style="0" width="11.9489795918367" collapsed="true"/>
+    <col min="3" max="3" hidden="false" style="0" width="6.1734693877551" collapsed="true"/>
     <col min="4" max="6" hidden="false" style="0" width="11.5204081632653" collapsed="true"/>
     <col min="7" max="7" hidden="false" style="0" width="18.1530612244898" collapsed="true"/>
     <col min="8" max="1025" hidden="false" style="0" width="11.5204081632653" collapsed="true"/>
@@ -1047,7 +1267,7 @@
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>3</v>
@@ -1056,52 +1276,50 @@
         <v>4</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.05" outlineLevel="0" r="2">
       <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="29" t="s">
-        <v>55</v>
-      </c>
-      <c r="C2" s="28" t="s">
-        <v>32</v>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5" t="s">
+        <v>14</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="3" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="G2" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="H2" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="H2" s="3" t="s">
-        <v>45</v>
-      </c>
       <c r="I2" s="3" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -1125,8 +1343,8 @@
   </sheetPr>
   <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100">
-      <selection activeCell="B2" activeCellId="0" pane="topLeft" sqref="B2"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="D1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100">
+      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1143,7 +1361,7 @@
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>3</v>
@@ -1152,25 +1370,25 @@
         <v>4</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="24.85" outlineLevel="0" r="2">
@@ -1178,32 +1396,32 @@
         <v>6</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="3" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="G2" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="H2" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="H2" s="3" t="s">
-        <v>45</v>
-      </c>
       <c r="I2" s="3" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>